<commit_message>
Updated Page 2 with SSE SZSE
</commit_message>
<xml_diff>
--- a/chatbook_charts.xlsx
+++ b/chatbook_charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuchen\Documents\GitHub\exchatbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93F71AD-1366-477C-B475-3D1D9211F433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68086BC-574E-4913-8130-EBFD2DD2DCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7155" yWindow="840" windowWidth="24360" windowHeight="19065" xr2:uid="{C77A330E-82A8-4DF5-9FBA-6BA8A73FFBAA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>IRR_Range</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>IRR &lt; 0%</t>
+  </si>
+  <si>
+    <t>SSE</t>
+  </si>
+  <si>
+    <t>SZSE</t>
   </si>
 </sst>
 </file>
@@ -195,7 +201,7 @@
                   <c:v>590907</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1988304</c:v>
+                  <c:v>2400254</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2068662</c:v>
@@ -266,7 +272,7 @@
                   <c:v>896087</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3432595</c:v>
+                  <c:v>4587549</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3774545</c:v>
@@ -337,7 +343,7 @@
                   <c:v>21996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60027</c:v>
+                  <c:v>82584</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>84511</c:v>
@@ -408,7 +414,7 @@
                   <c:v>4939</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20564</c:v>
+                  <c:v>26692</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>31430</c:v>
@@ -1179,16 +1185,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1513,7 +1519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE089598-4248-4448-BC8A-D558A289EBFB}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1524,9 +1530,10 @@
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1542,8 +1549,14 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1551,7 +1564,8 @@
         <v>590907</v>
       </c>
       <c r="C2" s="1">
-        <v>1988304</v>
+        <f>SUM(H2:I2)</f>
+        <v>2400254</v>
       </c>
       <c r="D2" s="1">
         <v>2068662</v>
@@ -1559,8 +1573,14 @@
       <c r="E2" s="1">
         <v>712546</v>
       </c>
+      <c r="H2" s="1">
+        <v>1988304</v>
+      </c>
+      <c r="I2" s="1">
+        <v>411950</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1568,7 +1588,8 @@
         <v>896087</v>
       </c>
       <c r="C3" s="1">
-        <v>3432595</v>
+        <f>SUM(H3:I3)</f>
+        <v>4587549</v>
       </c>
       <c r="D3" s="1">
         <v>3774545</v>
@@ -1576,8 +1597,14 @@
       <c r="E3" s="1">
         <v>1749129</v>
       </c>
+      <c r="H3" s="1">
+        <v>3432595</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1154954</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1585,7 +1612,8 @@
         <v>21996</v>
       </c>
       <c r="C4" s="1">
-        <v>60027</v>
+        <f>SUM(H4:I4)</f>
+        <v>82584</v>
       </c>
       <c r="D4" s="1">
         <v>84511</v>
@@ -1593,8 +1621,14 @@
       <c r="E4" s="1">
         <v>17601</v>
       </c>
+      <c r="H4" s="1">
+        <v>60027</v>
+      </c>
+      <c r="I4" s="1">
+        <v>22557</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1602,13 +1636,20 @@
         <v>4939</v>
       </c>
       <c r="C5" s="1">
-        <v>20564</v>
+        <f>SUM(H5:I5)</f>
+        <v>26692</v>
       </c>
       <c r="D5" s="1">
         <v>31430</v>
       </c>
       <c r="E5" s="1">
         <v>7579</v>
+      </c>
+      <c r="H5" s="1">
+        <v>20564</v>
+      </c>
+      <c r="I5" s="1">
+        <v>6128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added CDAX and N400 to Page 2
</commit_message>
<xml_diff>
--- a/chatbook_charts.xlsx
+++ b/chatbook_charts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuchen\Documents\GitHub\exchatbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\GitHub\exchatbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68086BC-574E-4913-8130-EBFD2DD2DCDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB2102C-ED50-4BF4-AD89-C1081E56AA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7155" yWindow="840" windowWidth="24360" windowHeight="19065" xr2:uid="{C77A330E-82A8-4DF5-9FBA-6BA8A73FFBAA}"/>
+    <workbookView xWindow="24420" yWindow="810" windowWidth="24360" windowHeight="19065" xr2:uid="{C77A330E-82A8-4DF5-9FBA-6BA8A73FFBAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>IRR_Range</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>SZSE</t>
+  </si>
+  <si>
+    <t>CDAX (DE)</t>
+  </si>
+  <si>
+    <t>JPX-Nikkei 400 (JP)</t>
   </si>
 </sst>
 </file>
@@ -101,17 +107,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -171,11 +180,239 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{212CE79D-B952-4AF3-A363-BA039DCA907E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{30FFAB6C-183D-4D81-A9D2-513C1D3E52B7}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{5AA76417-061F-44F3-8488-87E1A1844597}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DFE34852-AA9F-4795-A6B3-BEC93B7CCCD4}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{932877BC-64EC-4D13-83AF-5B5503F5A82D}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Hang Seng Composite (HK)</c:v>
                 </c:pt>
@@ -187,16 +424,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>FTSE All Share (UK)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CDAX (DE)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$E$2</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>590907</c:v>
                 </c:pt>
@@ -208,11 +448,40 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>712546</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>598847</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Sheet1!$B$8:$G$8</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>39.03%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>33.82%</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>34.71%</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>28.65%</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>36.23%</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>10.63%</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FBB1-4F99-865B-A08680096D11}"/>
             </c:ext>
@@ -242,11 +511,239 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{DED80882-07AE-4AC2-A152-1B3C57B2AA8A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{B97679B3-EE19-4B05-B3ED-35D549D636BB}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{CF6B790E-CEA0-49B8-B93F-89629FFF184B}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{358B0886-3402-4857-ADC2-00A34832BCC7}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0F27B54F-489F-4028-B7DD-F0AC8B0CC850}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000009-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Hang Seng Composite (HK)</c:v>
                 </c:pt>
@@ -258,16 +755,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>FTSE All Share (UK)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CDAX (DE)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$E$3</c:f>
+              <c:f>Sheet1!$B$3:$F$3</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>896087</c:v>
                 </c:pt>
@@ -279,11 +779,37 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1749129</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1035969</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Sheet1!$B$9:$F$9</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>59.19%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>64.64%</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>63.34%</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>70.33%</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>62.68%</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FBB1-4F99-865B-A08680096D11}"/>
             </c:ext>
@@ -313,11 +839,239 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{07C15BC8-8A1C-47CC-9AE6-465E21444478}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{E86C78F2-821E-4B12-936B-D3FE197C69ED}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C286A366-864C-4CC6-B31B-90D9D53606FF}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{37A9370D-E6FD-4532-9EE9-F28F896C5758}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D8F81B87-2E4C-4ADC-9131-FF1FFAB0E993}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="ctr"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Hang Seng Composite (HK)</c:v>
                 </c:pt>
@@ -329,16 +1083,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>FTSE All Share (UK)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CDAX (DE)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$E$4</c:f>
+              <c:f>Sheet1!$B$4:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>21996</c:v>
                 </c:pt>
@@ -350,11 +1107,37 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>17601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13059</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Sheet1!$B$10:$F$10</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>1.45%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.16%</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.42%</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.71%</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.79%</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-FBB1-4F99-865B-A08680096D11}"/>
             </c:ext>
@@ -384,11 +1167,239 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{8BDE6CC0-232F-4AFD-B37D-8C48A96D4A87}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{79E921E8-E55E-4C9D-85DC-7D76E81BBA49}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{3607D53E-5ED0-46F8-903D-16D6B05F2D5E}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000011-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{F078698B-ADCA-45AA-9949-710770F83298}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000012-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2E285DFF-4D16-4BC8-A034-995AB5B3BF2A}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-A827-49FA-B988-155C5CB27E41}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inBase"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$E$1</c:f>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Hang Seng Composite (HK)</c:v>
                 </c:pt>
@@ -400,16 +1411,19 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>FTSE All Share (UK)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>CDAX (DE)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$E$5</c:f>
+              <c:f>Sheet1!$B$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>4939</c:v>
                 </c:pt>
@@ -421,19 +1435,46 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7579</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>Sheet1!$B$11:$F$11</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.33%</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.38%</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.53%</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.30%</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.30%</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-FBB1-4F99-865B-A08680096D11}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1185,16 +2226,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1519,9 +2560,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE089598-4248-4448-BC8A-D558A289EBFB}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1530,10 +2573,12 @@
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1549,14 +2594,20 @@
       <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1564,7 +2615,7 @@
         <v>590907</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(H2:I2)</f>
+        <f>SUM(I2:J2)</f>
         <v>2400254</v>
       </c>
       <c r="D2" s="1">
@@ -1573,14 +2624,20 @@
       <c r="E2" s="1">
         <v>712546</v>
       </c>
-      <c r="H2" s="1">
+      <c r="F2" s="1">
+        <v>598847</v>
+      </c>
+      <c r="G2" s="1">
+        <v>211929</v>
+      </c>
+      <c r="I2" s="1">
         <v>1988304</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>411950</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1588,7 +2645,7 @@
         <v>896087</v>
       </c>
       <c r="C3" s="1">
-        <f>SUM(H3:I3)</f>
+        <f>SUM(I3:J3)</f>
         <v>4587549</v>
       </c>
       <c r="D3" s="1">
@@ -1597,14 +2654,20 @@
       <c r="E3" s="1">
         <v>1749129</v>
       </c>
-      <c r="H3" s="1">
+      <c r="F3" s="1">
+        <v>1035969</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1746857</v>
+      </c>
+      <c r="I3" s="1">
         <v>3432595</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>1154954</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1612,7 +2675,7 @@
         <v>21996</v>
       </c>
       <c r="C4" s="1">
-        <f>SUM(H4:I4)</f>
+        <f>SUM(I4:J4)</f>
         <v>82584</v>
       </c>
       <c r="D4" s="1">
@@ -1621,14 +2684,20 @@
       <c r="E4" s="1">
         <v>17601</v>
       </c>
-      <c r="H4" s="1">
+      <c r="F4" s="1">
+        <v>13059</v>
+      </c>
+      <c r="G4" s="1">
+        <v>26824</v>
+      </c>
+      <c r="I4" s="1">
         <v>60027</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>22557</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1636,7 +2705,7 @@
         <v>4939</v>
       </c>
       <c r="C5" s="1">
-        <f>SUM(H5:I5)</f>
+        <f>SUM(I5:J5)</f>
         <v>26692</v>
       </c>
       <c r="D5" s="1">
@@ -1645,11 +2714,121 @@
       <c r="E5" s="1">
         <v>7579</v>
       </c>
-      <c r="H5" s="1">
+      <c r="F5" s="1">
+        <v>5013</v>
+      </c>
+      <c r="G5" s="1">
+        <v>8164</v>
+      </c>
+      <c r="I5" s="1">
         <v>20564</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>6128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <f>B2/SUM(B$2:B$5)</f>
+        <v>0.39031354838965365</v>
+      </c>
+      <c r="C8" s="2">
+        <f>C2/SUM(C$2:C$5)</f>
+        <v>0.3382030832684827</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" ref="D8:G8" si="0">D2/SUM(D$2:D$5)</f>
+        <v>0.34714056438940599</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.28652494817751739</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.36230343495748046</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10629539757264364</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <f t="shared" ref="B9" si="1">B3/SUM(B$2:B$5)</f>
+        <v>0.59189499639679266</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" ref="C9:G12" si="2">C3/SUM(C$2:C$5)</f>
+        <v>0.64639959622825105</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.63340346640157286</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.70334981331842827</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.62676297486581067</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.87615597354564756</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <f t="shared" ref="B10" si="3">B4/SUM(B$2:B$5)</f>
+        <v>1.4529082935857626E-2</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1636336582980125E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="2"/>
+        <v>1.4181725307040536E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="2"/>
+        <v>7.077614094911042E-3</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="2"/>
+        <v>7.9007168059783851E-3</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3453881934461981E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <f t="shared" ref="B11" si="4">B5/SUM(B$2:B$5)</f>
+        <v>3.2623722776959816E-3</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="2"/>
+        <v>3.7609839202860781E-3</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="2"/>
+        <v>5.2742439019806183E-3</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="2"/>
+        <v>3.0476244091432753E-3</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="2"/>
+        <v>3.0328733707305033E-3</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>4.0947469472467791E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>